<commit_message>
QAPF map area5 + renaming notebooks area 2a+2b
</commit_message>
<xml_diff>
--- a/_CIPW/CIPW/AREA5/QAPF_counts.xlsx
+++ b/_CIPW/CIPW/AREA5/QAPF_counts.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -380,7 +380,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>177302</v>
+        <v>175292</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>quartz monzodiorite
+quartz monzogabbro</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>